<commit_message>
added 16 bit redpitaya in BOM
</commit_message>
<xml_diff>
--- a/Passepartout Large Boards.xlsx
+++ b/Passepartout Large Boards.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="199">
   <si>
     <t>FX6-60S-0.8SV(71)</t>
   </si>
@@ -605,6 +605,9 @@
   </si>
   <si>
     <t>https://ie.farnell.com/red-pitaya/izd0007/starter-kit-stemlab-125-14-data/dp/3935507?st=stemlab%2012</t>
+  </si>
+  <si>
+    <t>https://ie.farnell.com/red-pitaya/izd0021/standard-kit-sdrlab-122-16-data/dp/3935509</t>
   </si>
 </sst>
 </file>
@@ -3642,6 +3645,11 @@
         <v>197</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" s="136" t="s">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
@@ -3714,7 +3722,8 @@
     <hyperlink r:id="rId68" ref="A81"/>
     <hyperlink r:id="rId69" ref="A82"/>
     <hyperlink r:id="rId70" ref="A83"/>
+    <hyperlink r:id="rId71" ref="A84"/>
   </hyperlinks>
-  <drawing r:id="rId71"/>
+  <drawing r:id="rId72"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BOM has sma-bnc and 30mm fan
</commit_message>
<xml_diff>
--- a/Passepartout Large Boards.xlsx
+++ b/Passepartout Large Boards.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="202">
   <si>
     <t>FX6-60S-0.8SV(71)</t>
   </si>
@@ -608,6 +608,15 @@
   </si>
   <si>
     <t>https://ie.farnell.com/red-pitaya/izd0021/standard-kit-sdrlab-122-16-data/dp/3935509</t>
+  </si>
+  <si>
+    <t>https://ie.farnell.com/mcm/27-210/chassis-mount-female-solder-on/dp/2782149?st=bnc%20connector</t>
+  </si>
+  <si>
+    <t>https://ie.farnell.com/pro-signal/rw9-021/sma-male-to-bnc-female/dp/3384505?st=sma%20bnc</t>
+  </si>
+  <si>
+    <t>https://ie.farnell.com/wakefield-solutions/dc0301012u2b-2t0/axial-fan-30mm-12vdc-5-65cfm-31dba/dp/3481988?st=fan%2030%20mm</t>
   </si>
 </sst>
 </file>
@@ -3650,6 +3659,21 @@
         <v>198</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" s="136" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="136" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="136" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
@@ -3723,7 +3747,10 @@
     <hyperlink r:id="rId69" ref="A82"/>
     <hyperlink r:id="rId70" ref="A83"/>
     <hyperlink r:id="rId71" ref="A84"/>
+    <hyperlink r:id="rId72" ref="A85"/>
+    <hyperlink r:id="rId73" ref="A86"/>
+    <hyperlink r:id="rId74" ref="A87"/>
   </hyperlinks>
-  <drawing r:id="rId72"/>
+  <drawing r:id="rId75"/>
 </worksheet>
 </file>
</xml_diff>